<commit_message>
Gestion de asignaciones de cargos y gestión de tiempos laborados para estructuras orientada por proceso agregada
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/operationalsManagements/AssignedOperationalsManagements.xlsx
+++ b/src/main/resources/reports/operationalsManagements/AssignedOperationalsManagements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIS DOCUMENTOS\CIADTI\PROYECTOS\SERVICIOS\CARGA TRABAJO\ciadti-especifico-carga-trabajo-services\src\main\resources\reports\organizationChart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIS DOCUMENTOS\CIADTI\PROYECTOS\SERVICIOS\CARGA TRABAJO\ciadti-especifico-carga-trabajo-services\src\main\resources\reports\operationalsManagements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A93246E-9F5A-4A9D-A6E6-D6ED3A770D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF63D73-5BDF-4D2C-87D8-6762AC6531EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC55D6EF-68F2-426F-9839-57243A004983}"/>
   </bookViews>
@@ -650,7 +650,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -768,6 +768,13 @@
       <sz val="14"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Georgia Pro Black"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Garamond"/>
       <family val="1"/>
     </font>
   </fonts>
@@ -904,7 +911,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -983,6 +990,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1330,7 +1340,7 @@
   <dimension ref="B1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AQ5" sqref="AQ5"/>
+      <selection activeCell="AP4" sqref="AP4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1363,7 +1373,7 @@
       <c r="B5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="29"/>
     </row>
     <row r="6" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:11" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>